<commit_message>
manipulating excel files using write range and write cell
</commit_message>
<xml_diff>
--- a/Comparison Automation/NumbersList.xlsx
+++ b/Comparison Automation/NumbersList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Batches\211129-Illumina-UiPath\211129-RPA-Illumina-Training\Comparison Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625A9816-D1C9-4E17-BF63-92AA1091BA5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072FD79A-29D2-43EB-AFC9-E406A4C0ADC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -363,7 +363,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>